<commit_message>
Wing Servo holders cutted.
</commit_message>
<xml_diff>
--- a/Course Materials/Cost Analysis.xlsx
+++ b/Course Materials/Cost Analysis.xlsx
@@ -198,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -236,15 +236,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -268,10 +259,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -279,8 +270,68 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -288,8 +339,23 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -299,25 +365,36 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -329,58 +406,25 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="double">
+      <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -390,39 +434,40 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="İyi" xfId="1" builtinId="26"/>
@@ -709,7 +754,7 @@
   <dimension ref="B1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,23 +762,23 @@
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="7.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="7" customWidth="1"/>
     <col min="5" max="5" width="10.21875" customWidth="1"/>
     <col min="6" max="6" width="80" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -741,314 +786,314 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="14">
         <v>1</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="15">
         <v>599</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="15">
         <f>C3*D3</f>
         <v>599</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="17">
         <v>1</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="18">
         <v>300</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="19">
         <f t="shared" ref="E4:E22" si="0">C4*D4</f>
         <v>300</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="18">
         <v>313.73</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="19">
         <f t="shared" si="0"/>
         <v>313.73</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="17">
         <v>1</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="18">
         <v>500</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="19">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="17">
         <v>3</v>
       </c>
-      <c r="D7" s="16">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="20" t="s">
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="17">
         <v>3</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="18">
         <v>524.16</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="19">
         <f t="shared" si="0"/>
         <v>1572.48</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="17">
         <v>1</v>
       </c>
-      <c r="D9" s="16">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="18">
+        <v>0</v>
+      </c>
+      <c r="E9" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="17">
         <v>2</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="18">
         <v>643.97</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="19">
         <f t="shared" si="0"/>
         <v>1287.94</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="21" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="17">
         <v>5</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="18">
         <v>106.5</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="19">
         <f t="shared" si="0"/>
         <v>532.5</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="17">
         <v>1</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="18">
         <v>2140</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="19">
         <f t="shared" si="0"/>
         <v>2140</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="17">
         <v>3</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="18">
         <v>54.42</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="19">
         <f t="shared" si="0"/>
         <v>163.26</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="18">
         <v>6770</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="19">
         <f t="shared" si="0"/>
         <v>6770</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="17">
         <v>1</v>
       </c>
-      <c r="D15" s="16">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="D15" s="18">
+        <v>0</v>
+      </c>
+      <c r="E15" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="2"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="11"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="11">
         <f>SUM(E3:E22)</f>
         <v>14178.91</v>
       </c>
@@ -1066,6 +1111,6 @@
     <hyperlink ref="F14" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fuselage covers are desiged.
</commit_message>
<xml_diff>
--- a/Course Materials/Cost Analysis.xlsx
+++ b/Course Materials/Cost Analysis.xlsx
@@ -459,7 +459,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -468,6 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="İyi" xfId="1" builtinId="26"/>
@@ -754,7 +754,7 @@
   <dimension ref="B1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,285 +799,285 @@
         <f>C3*D3</f>
         <v>599</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>1</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>300</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <f t="shared" ref="E4:E22" si="0">C4*D4</f>
         <v>300</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>313.73</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <f t="shared" si="0"/>
         <v>313.73</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>500</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>3</v>
       </c>
-      <c r="D7" s="18">
-        <v>0</v>
-      </c>
-      <c r="E7" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="23" t="s">
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>3</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>524.16</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>1572.48</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>1</v>
       </c>
-      <c r="D9" s="18">
-        <v>0</v>
-      </c>
-      <c r="E9" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="23" t="s">
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>2</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>643.97</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <f t="shared" si="0"/>
         <v>1287.94</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>5</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>106.5</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <f t="shared" si="0"/>
         <v>532.5</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>2140</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <f t="shared" si="0"/>
         <v>2140</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>3</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>54.42</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <f t="shared" si="0"/>
         <v>163.26</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>1</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>6770</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <f t="shared" si="0"/>
         <v>6770</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>1</v>
       </c>
-      <c r="D15" s="18">
-        <v>0</v>
-      </c>
-      <c r="E15" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="24" t="s">
+      <c r="D15" s="17">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="22"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="22"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="20"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="22"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="22"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="20"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="22"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="20"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="22"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>

</xml_diff>